<commit_message>
specific activity analysis 4
</commit_message>
<xml_diff>
--- a/wet_lab_analysis/activity_assay/activity_summary_activity_master.xlsx
+++ b/wet_lab_analysis/activity_assay/activity_summary_activity_master.xlsx
@@ -685,7 +685,7 @@
         <v>0.9982291666666667</v>
       </c>
       <c r="G9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -712,7 +712,7 @@
         <v>0.9980607756897242</v>
       </c>
       <c r="G10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -739,7 +739,7 @@
         <v>0.9980311446141638</v>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -766,7 +766,7 @@
         <v>0.9976713532513182</v>
       </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -793,7 +793,7 @@
         <v>0.9957860615883305</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -820,7 +820,7 @@
         <v>0.995617283950617</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -847,7 +847,7 @@
         <v>0.9956172839506172</v>
       </c>
       <c r="G15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -874,7 +874,7 @@
         <v>0.9952885747938753</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -901,7 +901,7 @@
         <v>0.9956721180694057</v>
       </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -928,7 +928,7 @@
         <v>0.9963762673676304</v>
       </c>
       <c r="G18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -955,7 +955,7 @@
         <v>0.9963762673676304</v>
       </c>
       <c r="G19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -982,7 +982,7 @@
         <v>0.9965843429636533</v>
       </c>
       <c r="G20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1009,7 +1009,7 @@
         <v>0.9979010768388393</v>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1036,7 +1036,7 @@
         <v>0.998061144754835</v>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1063,7 +1063,7 @@
         <v>0.9986842105263158</v>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1252,7 +1252,7 @@
         <v>0.9988787483702738</v>
       </c>
       <c r="G30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1306,7 +1306,7 @@
         <v>0.9989630044843052</v>
       </c>
       <c r="G32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1441,7 +1441,7 @@
         <v>0.9989630044843048</v>
       </c>
       <c r="G37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1495,7 +1495,7 @@
         <v>0.9988787483702738</v>
       </c>
       <c r="G39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1603,7 +1603,7 @@
         <v>0.9988787483702739</v>
       </c>
       <c r="G43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1846,7 +1846,7 @@
         <v>0.9989630044843051</v>
       </c>
       <c r="G52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2089,7 +2089,7 @@
         <v>0.995862910381544</v>
       </c>
       <c r="G61" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -2116,7 +2116,7 @@
         <v>0.9971265560165976</v>
       </c>
       <c r="G62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -2143,7 +2143,7 @@
         <v>0.9971895292207792</v>
       </c>
       <c r="G63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -2170,7 +2170,7 @@
         <v>0.9974880857823669</v>
       </c>
       <c r="G64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -2197,7 +2197,7 @@
         <v>0.997421816827997</v>
       </c>
       <c r="G65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2224,7 +2224,7 @@
         <v>0.998832271762208</v>
       </c>
       <c r="G66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2251,7 +2251,7 @@
         <v>0.9981738683127572</v>
       </c>
       <c r="G67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2278,7 +2278,7 @@
         <v>0.9981738683127572</v>
       </c>
       <c r="G68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2305,7 +2305,7 @@
         <v>0.9986802286482852</v>
       </c>
       <c r="G69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2332,7 +2332,7 @@
         <v>0.9986802286482852</v>
       </c>
       <c r="G70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2359,7 +2359,7 @@
         <v>0.9981738683127571</v>
       </c>
       <c r="G71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2386,7 +2386,7 @@
         <v>0.9981738683127575</v>
       </c>
       <c r="G72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2413,7 +2413,7 @@
         <v>0.9988322717622079</v>
       </c>
       <c r="G73" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2440,7 +2440,7 @@
         <v>0.998811226313908</v>
       </c>
       <c r="G74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2494,7 +2494,7 @@
         <v>0.998832271762208</v>
       </c>
       <c r="G76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2575,7 +2575,7 @@
         <v>0.998832271762208</v>
       </c>
       <c r="G79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2629,7 +2629,7 @@
         <v>0.9988112263139077</v>
       </c>
       <c r="G81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2656,7 +2656,7 @@
         <v>0.9988322717622081</v>
       </c>
       <c r="G82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2683,7 +2683,7 @@
         <v>0.9988112263139076</v>
       </c>
       <c r="G83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2764,7 +2764,7 @@
         <v>0.9989093959731543</v>
       </c>
       <c r="G86" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2791,7 +2791,7 @@
         <v>0.9985675182481751</v>
       </c>
       <c r="G87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2818,7 +2818,7 @@
         <v>0.998567518248175</v>
       </c>
       <c r="G88" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -2845,7 +2845,7 @@
         <v>0.9989093959731543</v>
       </c>
       <c r="G89" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -2926,7 +2926,7 @@
         <v>0.9989093959731544</v>
       </c>
       <c r="G92" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2953,7 +2953,7 @@
         <v>0.9987338156892612</v>
       </c>
       <c r="G93" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2980,7 +2980,7 @@
         <v>0.9984180790960453</v>
       </c>
       <c r="G94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -3007,7 +3007,7 @@
         <v>0.9987338156892613</v>
       </c>
       <c r="G95" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -3034,7 +3034,7 @@
         <v>0.9989093959731543</v>
       </c>
       <c r="G96" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -3115,7 +3115,7 @@
         <v>0.9988112263139077</v>
       </c>
       <c r="G99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -3142,7 +3142,7 @@
         <v>0.9988322717622079</v>
       </c>
       <c r="G100" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -3169,7 +3169,7 @@
         <v>0.9988112263139077</v>
       </c>
       <c r="G101" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -3250,7 +3250,7 @@
         <v>0.9989093959731544</v>
       </c>
       <c r="G104" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -3277,7 +3277,7 @@
         <v>0.9985675182481754</v>
       </c>
       <c r="G105" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -3304,7 +3304,7 @@
         <v>0.9985675182481751</v>
       </c>
       <c r="G106" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -3331,7 +3331,7 @@
         <v>0.9989093959731544</v>
       </c>
       <c r="G107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -3358,7 +3358,7 @@
         <v>0.998338081671415</v>
       </c>
       <c r="G108" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -4627,7 +4627,7 @@
         <v>0.9989261947973382</v>
       </c>
       <c r="G155" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -4654,7 +4654,7 @@
         <v>0.9986842105263158</v>
       </c>
       <c r="G156" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -4708,7 +4708,7 @@
         <v>0.9983822509822049</v>
       </c>
       <c r="G158" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -4762,7 +4762,7 @@
         <v>0.9987641668676152</v>
       </c>
       <c r="G160" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -4789,7 +4789,7 @@
         <v>0.9969833296533451</v>
       </c>
       <c r="G161" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -4816,7 +4816,7 @@
         <v>0.9989150255288112</v>
       </c>
       <c r="G162" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -5005,7 +5005,7 @@
         <v>0.9988385851289077</v>
       </c>
       <c r="G169" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -5032,7 +5032,7 @@
         <v>0.9989018087855297</v>
       </c>
       <c r="G170" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -5059,7 +5059,7 @@
         <v>0.9987936064178924</v>
       </c>
       <c r="G171" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172">
@@ -6787,7 +6787,7 @@
         <v>0.9989722507708119</v>
       </c>
       <c r="G235" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236">
@@ -7084,7 +7084,7 @@
         <v>0.9964694656488551</v>
       </c>
       <c r="G246" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247">
@@ -7111,7 +7111,7 @@
         <v>0.9972332015810276</v>
       </c>
       <c r="G247" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248">
@@ -7138,7 +7138,7 @@
         <v>0.9963099630996308</v>
       </c>
       <c r="G248" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249">
@@ -7165,7 +7165,7 @@
         <v>0.9975778546712802</v>
       </c>
       <c r="G249" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250">
@@ -7192,7 +7192,7 @@
         <v>0.9975941422594141</v>
       </c>
       <c r="G250" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251">
@@ -7219,7 +7219,7 @@
         <v>0.9975941422594142</v>
       </c>
       <c r="G251" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252">
@@ -7246,7 +7246,7 @@
         <v>0.9968703976435934</v>
       </c>
       <c r="G252" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253">
@@ -7327,7 +7327,7 @@
         <v>0.9987432065217391</v>
       </c>
       <c r="G255" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256">
@@ -7354,7 +7354,7 @@
         <v>0.9988589567604668</v>
       </c>
       <c r="G256" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257">
@@ -7408,7 +7408,7 @@
         <v>0.9988589567604667</v>
       </c>
       <c r="G258" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259">
@@ -7435,7 +7435,7 @@
         <v>0.9987432065217391</v>
       </c>
       <c r="G259" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260">
@@ -7489,7 +7489,7 @@
         <v>0.9986684420772303</v>
       </c>
       <c r="G261" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262">
@@ -7516,7 +7516,7 @@
         <v>0.9987063282794989</v>
       </c>
       <c r="G262" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263">
@@ -7543,7 +7543,7 @@
         <v>0.9982800387596898</v>
       </c>
       <c r="G263" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264">
@@ -7570,7 +7570,7 @@
         <v>0.9989642184557439</v>
       </c>
       <c r="G264" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265">
@@ -7597,7 +7597,7 @@
         <v>0.9989642184557439</v>
       </c>
       <c r="G265" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266">
@@ -7624,7 +7624,7 @@
         <v>0.9989664283493939</v>
       </c>
       <c r="G266" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="267">
@@ -7678,7 +7678,7 @@
         <v>0.9989642184557438</v>
       </c>
       <c r="G268" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269">
@@ -7732,7 +7732,7 @@
         <v>0.9989664283493938</v>
       </c>
       <c r="G270" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271">
@@ -7759,7 +7759,7 @@
         <v>0.9989642184557438</v>
       </c>
       <c r="G271" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="272">
@@ -7786,7 +7786,7 @@
         <v>0.9989642184557438</v>
       </c>
       <c r="G272" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273">
@@ -7813,7 +7813,7 @@
         <v>0.9989664283493939</v>
       </c>
       <c r="G273" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274">
@@ -7948,7 +7948,7 @@
         <v>0.9972226298796593</v>
       </c>
       <c r="G278" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279">
@@ -9298,7 +9298,7 @@
         <v>0.9954301075268815</v>
       </c>
       <c r="G328" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329">
@@ -10108,7 +10108,7 @@
         <v>0.9957704741379315</v>
       </c>
       <c r="G358" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="359">
@@ -10135,7 +10135,7 @@
         <v>0.9956145251396648</v>
       </c>
       <c r="G359" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="360">
@@ -10270,7 +10270,7 @@
         <v>0.9983667409057164</v>
       </c>
       <c r="G364" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="365">
@@ -10351,7 +10351,7 @@
         <v>0.9989776632302406</v>
       </c>
       <c r="G367" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="368">
@@ -10405,7 +10405,7 @@
         <v>0.9989776632302406</v>
       </c>
       <c r="G369" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="370">
@@ -10432,7 +10432,7 @@
         <v>0.9974424322379467</v>
       </c>
       <c r="G370" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="371">
@@ -10459,7 +10459,7 @@
         <v>0.9960884778805296</v>
       </c>
       <c r="G371" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372">
@@ -10486,7 +10486,7 @@
         <v>0.9956394575910659</v>
       </c>
       <c r="G372" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="373">
@@ -10756,7 +10756,7 @@
         <v>0.9989798109965635</v>
       </c>
       <c r="G382" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="383">
@@ -10783,7 +10783,7 @@
         <v>0.9984069815763957</v>
       </c>
       <c r="G383" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384">
@@ -10864,7 +10864,7 @@
         <v>0.9952897808724143</v>
       </c>
       <c r="G386" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="387">
@@ -10891,7 +10891,7 @@
         <v>0.9969808649809626</v>
       </c>
       <c r="G387" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="388">
@@ -10918,7 +10918,7 @@
         <v>0.9978788167031294</v>
       </c>
       <c r="G388" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="389">
@@ -10945,7 +10945,7 @@
         <v>0.9958073148974129</v>
       </c>
       <c r="G389" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390">
@@ -11026,7 +11026,7 @@
         <v>0.9978728666831561</v>
       </c>
       <c r="G392" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="393">
@@ -11107,7 +11107,7 @@
         <v>0.9978309111478547</v>
       </c>
       <c r="G395" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="396">
@@ -11242,7 +11242,7 @@
         <v>0.9988559542381696</v>
       </c>
       <c r="G400" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="401">
@@ -11944,7 +11944,7 @@
         <v>0.9968942250446517</v>
       </c>
       <c r="G426" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="427">
@@ -11971,7 +11971,7 @@
         <v>0.9979507326396264</v>
       </c>
       <c r="G427" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="428">
@@ -11998,7 +11998,7 @@
         <v>0.998895468002733</v>
       </c>
       <c r="G428" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="429">
@@ -12869,13 +12869,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.000262536231884058</v>
+        <v>-0.0002504444444444444</v>
       </c>
       <c r="E2" t="n">
-        <v>2.009326488650234e-05</v>
+        <v>9.583937179043098e-06</v>
       </c>
     </row>
     <row r="3">
@@ -12890,13 +12890,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0002121040189125294</v>
+        <v>-0.0002122222222222217</v>
       </c>
       <c r="E3" t="n">
-        <v>5.391107693412507e-06</v>
+        <v>2.484519974999497e-06</v>
       </c>
     </row>
     <row r="4">
@@ -12911,13 +12911,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0003014255765199161</v>
+        <v>-0.0003033101851851852</v>
       </c>
       <c r="E4" t="n">
-        <v>1.554263818039992e-05</v>
+        <v>1.346480243050236e-05</v>
       </c>
     </row>
     <row r="5">
@@ -12932,13 +12932,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0003552688172043011</v>
+        <v>-0.0003524358974358975</v>
       </c>
       <c r="E5" t="n">
-        <v>1.449252472669434e-05</v>
+        <v>1.37299252775185e-05</v>
       </c>
     </row>
     <row r="6">
@@ -12953,13 +12953,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0004447798742138363</v>
+        <v>-0.0004456410256410255</v>
       </c>
       <c r="E6" t="n">
-        <v>4.355802890854227e-05</v>
+        <v>4.352567773957973e-05</v>
       </c>
     </row>
     <row r="7">
@@ -12974,13 +12974,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0002190476190476191</v>
+        <v>-0.0002211111111111107</v>
       </c>
       <c r="E7" t="n">
-        <v>1.040923771372336e-05</v>
+        <v>4.006168083848449e-06</v>
       </c>
     </row>
     <row r="8">
@@ -12995,13 +12995,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0002948299319727891</v>
+        <v>-0.0002940046296296296</v>
       </c>
       <c r="E8" t="n">
-        <v>1.730166159938623e-05</v>
+        <v>1.649875226503966e-05</v>
       </c>
     </row>
     <row r="9">
@@ -13016,14 +13016,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-0.0002225925925925921</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3.095640547254345e-05</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -13037,13 +13033,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0003734640522875819</v>
+        <v>-0.0003658333333333336</v>
       </c>
       <c r="E10" t="n">
-        <v>2.332207120970873e-05</v>
+        <v>1.73449925174999e-05</v>
       </c>
     </row>
     <row r="11">
@@ -13058,13 +13054,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.0004455913978494621</v>
+        <v>-0.0004463218390804597</v>
       </c>
       <c r="E11" t="n">
-        <v>1.347736976919004e-05</v>
+        <v>1.363360311703455e-05</v>
       </c>
     </row>
     <row r="12">
@@ -13079,13 +13075,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.000387003367003367</v>
+        <v>-0.0003863703703703704</v>
       </c>
       <c r="E12" t="n">
-        <v>1.436389050463296e-05</v>
+        <v>1.451530576697952e-05</v>
       </c>
     </row>
   </sheetData>
@@ -13157,7 +13153,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.000262536231884058</v>
+        <v>-0.0002504444444444444</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -13166,7 +13162,7 @@
         <v>0.01</v>
       </c>
       <c r="G2" t="n">
-        <v>-10.13001537816301</v>
+        <v>-9.663451232583064</v>
       </c>
     </row>
     <row r="3">
@@ -13182,7 +13178,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0002121040189125294</v>
+        <v>-0.0002122222222222217</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -13191,7 +13187,7 @@
         <v>0.01</v>
       </c>
       <c r="G3" t="n">
-        <v>-8.184077900161908</v>
+        <v>-8.188638799571258</v>
       </c>
     </row>
     <row r="4">
@@ -13207,7 +13203,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0003014255765199161</v>
+        <v>-0.0003033101851851852</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -13216,7 +13212,7 @@
         <v>0.01</v>
       </c>
       <c r="G4" t="n">
-        <v>-11.63056886893567</v>
+        <v>-11.70328688817435</v>
       </c>
     </row>
     <row r="5">
@@ -13232,7 +13228,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0003552688172043011</v>
+        <v>-0.0003524358974358975</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -13241,7 +13237,7 @@
         <v>0.01</v>
       </c>
       <c r="G5" t="n">
-        <v>-13.7081215641531</v>
+        <v>-13.5988127627999</v>
       </c>
     </row>
     <row r="6">
@@ -13257,7 +13253,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0004447798742138363</v>
+        <v>-0.0004456410256410255</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -13266,7 +13262,7 @@
         <v>0.1</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.716192440696475</v>
+        <v>-1.719515211476625</v>
       </c>
     </row>
     <row r="7">
@@ -13282,7 +13278,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0002190476190476191</v>
+        <v>-0.0002211111111111107</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -13291,7 +13287,7 @@
         <v>0.01</v>
       </c>
       <c r="G7" t="n">
-        <v>-8.451998162609097</v>
+        <v>-8.531618435155396</v>
       </c>
     </row>
     <row r="8">
@@ -13307,7 +13303,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0002948299319727891</v>
+        <v>-0.0002940046296296296</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -13316,7 +13312,7 @@
         <v>0.01</v>
       </c>
       <c r="G8" t="n">
-        <v>-11.37607454557386</v>
+        <v>-11.34423008217221</v>
       </c>
     </row>
     <row r="9">
@@ -13329,20 +13325,14 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-0.0002225925925925921</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>0.01</v>
       </c>
-      <c r="G9" t="n">
-        <v>-8.588781707752752</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -13357,7 +13347,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0003734640522875819</v>
+        <v>-0.0003658333333333336</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -13366,7 +13356,7 @@
         <v>0.1</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.441018851270413</v>
+        <v>-1.411575562700966</v>
       </c>
     </row>
     <row r="11">
@@ -13382,7 +13372,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.0004455913978494621</v>
+        <v>-0.0004463218390804597</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -13391,7 +13381,7 @@
         <v>0.01</v>
       </c>
       <c r="G11" t="n">
-        <v>-17.19323721605642</v>
+        <v>-17.22142144361903</v>
       </c>
     </row>
     <row r="12">
@@ -13407,7 +13397,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.000387003367003367</v>
+        <v>-0.0003863703703703704</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -13416,7 +13406,7 @@
         <v>0.01</v>
       </c>
       <c r="G12" t="n">
-        <v>-14.932605800773</v>
+        <v>-14.9081814933905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
specific activity analysis 6
</commit_message>
<xml_diff>
--- a/wet_lab_analysis/activity_assay/activity_summary_activity_master.xlsx
+++ b/wet_lab_analysis/activity_assay/activity_summary_activity_master.xlsx
@@ -13162,7 +13162,7 @@
         <v>0.01</v>
       </c>
       <c r="G2" t="n">
-        <v>-9.663451232583064</v>
+        <v>9.663451232583064</v>
       </c>
     </row>
     <row r="3">
@@ -13187,7 +13187,7 @@
         <v>0.01</v>
       </c>
       <c r="G3" t="n">
-        <v>-8.188638799571258</v>
+        <v>8.188638799571258</v>
       </c>
     </row>
     <row r="4">
@@ -13212,7 +13212,7 @@
         <v>0.01</v>
       </c>
       <c r="G4" t="n">
-        <v>-11.70328688817435</v>
+        <v>11.70328688817435</v>
       </c>
     </row>
     <row r="5">
@@ -13237,7 +13237,7 @@
         <v>0.01</v>
       </c>
       <c r="G5" t="n">
-        <v>-13.5988127627999</v>
+        <v>13.5988127627999</v>
       </c>
     </row>
     <row r="6">
@@ -13262,7 +13262,7 @@
         <v>0.1</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.719515211476625</v>
+        <v>1.719515211476625</v>
       </c>
     </row>
     <row r="7">
@@ -13287,7 +13287,7 @@
         <v>0.01</v>
       </c>
       <c r="G7" t="n">
-        <v>-8.531618435155396</v>
+        <v>8.531618435155396</v>
       </c>
     </row>
     <row r="8">
@@ -13312,7 +13312,7 @@
         <v>0.01</v>
       </c>
       <c r="G8" t="n">
-        <v>-11.34423008217221</v>
+        <v>11.34423008217221</v>
       </c>
     </row>
     <row r="9">
@@ -13356,7 +13356,7 @@
         <v>0.1</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.411575562700966</v>
+        <v>1.411575562700966</v>
       </c>
     </row>
     <row r="11">
@@ -13381,7 +13381,7 @@
         <v>0.01</v>
       </c>
       <c r="G11" t="n">
-        <v>-17.22142144361903</v>
+        <v>17.22142144361903</v>
       </c>
     </row>
     <row r="12">
@@ -13406,7 +13406,7 @@
         <v>0.01</v>
       </c>
       <c r="G12" t="n">
-        <v>-14.9081814933905</v>
+        <v>14.9081814933905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>